<commit_message>
Se elimina hoja 4 de pruebas
</commit_message>
<xml_diff>
--- a/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
+++ b/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\Carg_Masiva\doc_masiva\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\doc_masiva\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA8C9AF-97C1-42BB-BC99-AE2792A54296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29217E1-008A-4700-B503-ACD640C72D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
+    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1772,7 +1771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267302D1-1807-4EAE-9A86-AD84416E3204}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -2122,16 +2121,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBED7625-E166-4B42-BEAA-D080C8DF683A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Se sube el archivo con el plan de restructuración del módulo para documentación masiva sin factura.
Se desarrollan todas las funciones de la sección de validaciones y se actualiza archivo excel de seguimiento.
Aquí surge la necesidad de desarrollar una función adicional que se encargará de obtener el tipo de tarifa que tiene configurado un cliente: tipo_tarifa_cliente; la cual queda pendiente de implementar.
</commit_message>
<xml_diff>
--- a/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
+++ b/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\doc_masiva\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29217E1-008A-4700-B503-ACD640C72D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71B05A1-0A7B-4A77-9434-88134F773BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t xml:space="preserve">Inicializar variables </t>
   </si>
@@ -1771,8 +1771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267302D1-1807-4EAE-9A86-AD84416E3204}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,7 +1885,9 @@
       <c r="C10" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
@@ -1897,7 +1899,9 @@
       <c r="C11" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
@@ -1909,7 +1913,9 @@
       <c r="C12" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
@@ -1921,7 +1927,9 @@
       <c r="C13" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="32"/>
+      <c r="D13" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
@@ -1933,7 +1941,9 @@
       <c r="C14" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="32"/>
+      <c r="D14" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
@@ -1945,7 +1955,9 @@
       <c r="C15" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="29" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24">
@@ -1957,7 +1969,9 @@
       <c r="C16" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="35" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="20">

</xml_diff>

<commit_message>
Se agregó la función obtener destinatario
</commit_message>
<xml_diff>
--- a/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
+++ b/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\doc_masiva\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\Carg_Masiva\doc_masiva\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1309D4-338D-4572-A393-8B6B91EFDE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEC8BD0-E536-4659-9953-79D63674D5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
   <si>
     <t xml:space="preserve">Inicializar variables </t>
   </si>
@@ -1039,6 +1039,9 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1050,9 +1053,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1468,7 +1468,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1479,7 +1479,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1493,7 +1493,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="34" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1532,7 +1532,7 @@
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1562,11 +1562,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1647,7 +1647,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1658,7 +1658,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="7" t="s">
         <v>52</v>
       </c>
@@ -1726,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267302D1-1807-4EAE-9A86-AD84416E3204}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1740,10 +1740,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -1938,7 +1938,7 @@
       <c r="C17" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="33" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1994,7 +1994,9 @@
       <c r="C21" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="31"/>
+      <c r="D21" s="32" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
@@ -2102,7 +2104,7 @@
       <c r="C30" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="33" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se crea funcion para validar que la cantidad de NUI's disponibles sea mayor o igual que los NUI's necesarios por el LayOut
</commit_message>
<xml_diff>
--- a/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
+++ b/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\Carg_Masiva\doc_masiva\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\doc_masiva\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAEC8BD0-E536-4659-9953-79D63674D5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E423C32-9482-4B18-B5C1-EA6F2D05FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
+    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="119">
   <si>
     <t xml:space="preserve">Inicializar variables </t>
   </si>
@@ -632,6 +632,12 @@
   </si>
   <si>
     <t>Tipo de Tarifa por número de cuenta: 1.-Peso/Volumen | 2.-Caja/Tarima | 3.-Bulto Constitutivo | 4.-Solo Tarima</t>
+  </si>
+  <si>
+    <t>Cantidad de NUI's reservados (estatus =&gt; 3) con los que cuenta el Cliente</t>
+  </si>
+  <si>
+    <t>obtener_nuis_disponibles()</t>
   </si>
 </sst>
 </file>
@@ -714,7 +720,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -750,6 +756,12 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -943,7 +955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1053,6 +1065,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1724,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267302D1-1807-4EAE-9A86-AD84416E3204}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2008,19 +2035,21 @@
       <c r="C22" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="33" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="39">
         <v>19</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="30"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
@@ -2105,6 +2134,20 @@
         <v>116</v>
       </c>
       <c r="D30" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="23">
+        <v>27</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="42" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2113,5 +2156,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se integró celda para saber que tipo de dato retorna cada función / se creó el módulo de doc_masiva_sin_factura.bas
</commit_message>
<xml_diff>
--- a/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
+++ b/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\doc_masiva\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectosGITHUB\Carg_Masiva\doc_masiva\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E423C32-9482-4B18-B5C1-EA6F2D05FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C859736A-A723-4EA7-ACB0-94661794A773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="128">
   <si>
     <t xml:space="preserve">Inicializar variables </t>
   </si>
@@ -638,6 +638,33 @@
   </si>
   <si>
     <t>obtener_nuis_disponibles()</t>
+  </si>
+  <si>
+    <t>TIPO DATO O VALOR QUE RETORNA CADA FUNCION</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>STRING "S" / "N"</t>
+  </si>
+  <si>
+    <t>STRING "PREPAGADO" / "POR COBRAR"</t>
+  </si>
+  <si>
+    <t>STRING TEXTO DEL CAMPO</t>
+  </si>
+  <si>
+    <t>STRING CANTIDAD</t>
+  </si>
+  <si>
+    <t>STRING CCLCLAVE Y DIECLAVE</t>
+  </si>
+  <si>
+    <t>STRING CCLCLAVE</t>
+  </si>
+  <si>
+    <t>STRING ID_TIPO_TARIFA</t>
   </si>
 </sst>
 </file>
@@ -1054,6 +1081,21 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1065,21 +1107,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1495,7 +1522,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1506,7 +1533,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1520,7 +1547,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="40" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1531,7 +1558,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1575,7 @@
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="39" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1559,7 +1586,7 @@
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1589,11 +1616,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1674,7 +1701,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1685,7 +1712,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="7" t="s">
         <v>52</v>
       </c>
@@ -1751,33 +1778,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267302D1-1807-4EAE-9A86-AD84416E3204}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="10" customWidth="1"/>
     <col min="2" max="2" width="33.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="104.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="28"/>
-    <col min="5" max="16384" width="11.42578125" style="10"/>
+    <col min="3" max="3" width="47.140625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="90.28515625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="37"/>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>110</v>
       </c>
@@ -1785,25 +1813,29 @@
         <v>111</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>1</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="29"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <v>2</v>
       </c>
@@ -1811,13 +1843,16 @@
         <v>60</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="E6" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="22">
         <v>3</v>
       </c>
@@ -1825,13 +1860,16 @@
         <v>61</v>
       </c>
       <c r="C7" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="E7" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="24">
         <v>4</v>
       </c>
@@ -1839,25 +1877,29 @@
         <v>62</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="E8" s="32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>5</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="29"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <v>6</v>
       </c>
@@ -1865,13 +1907,16 @@
         <v>64</v>
       </c>
       <c r="C10" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="E10" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <v>7</v>
       </c>
@@ -1879,13 +1924,16 @@
         <v>66</v>
       </c>
       <c r="C11" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>8</v>
       </c>
@@ -1893,13 +1941,16 @@
         <v>79</v>
       </c>
       <c r="C12" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="E12" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
         <v>9</v>
       </c>
@@ -1907,13 +1958,16 @@
         <v>81</v>
       </c>
       <c r="C13" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="E13" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>10</v>
       </c>
@@ -1921,13 +1975,16 @@
         <v>83</v>
       </c>
       <c r="C14" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="E14" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>11</v>
       </c>
@@ -1935,13 +1992,16 @@
         <v>69</v>
       </c>
       <c r="C15" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="E15" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24">
         <v>12</v>
       </c>
@@ -1949,13 +2009,16 @@
         <v>72</v>
       </c>
       <c r="C16" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="E16" s="32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>13</v>
       </c>
@@ -1963,13 +2026,16 @@
         <v>89</v>
       </c>
       <c r="C17" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="E17" s="33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>14</v>
       </c>
@@ -1977,41 +2043,50 @@
         <v>85</v>
       </c>
       <c r="C18" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="27" t="s">
+      <c r="E18" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22">
         <v>15</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="E19" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <v>16</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="E20" s="27" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24">
         <v>17</v>
       </c>
@@ -2019,13 +2094,16 @@
         <v>92</v>
       </c>
       <c r="C21" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="E21" s="32" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>18</v>
       </c>
@@ -2033,97 +2111,107 @@
         <v>94</v>
       </c>
       <c r="C22" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="E22" s="33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="35">
         <v>19</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="41"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="37"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
         <v>20</v>
       </c>
       <c r="B24" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="23"/>
+      <c r="D24" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="30"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="30"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="22">
         <v>21</v>
       </c>
       <c r="B25" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="30"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="30"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <v>22</v>
       </c>
       <c r="B26" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="23"/>
+      <c r="D26" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="30"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="30"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24">
         <v>23</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="25"/>
+      <c r="D27" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="31"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="31"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>24</v>
       </c>
       <c r="B28" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="26"/>
+      <c r="D28" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="29"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="29"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24">
         <v>25</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="25"/>
+      <c r="D29" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="31"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="31"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <v>26</v>
       </c>
@@ -2131,13 +2219,16 @@
         <v>115</v>
       </c>
       <c r="C30" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="33" t="s">
+      <c r="E30" s="33" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>27</v>
       </c>
@@ -2145,9 +2236,12 @@
         <v>118</v>
       </c>
       <c r="C31" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="E31" s="38" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se suben archivos actualizados
</commit_message>
<xml_diff>
--- a/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
+++ b/Documentacion/Plan Restructuración Modulo Documentación Masiva-SIN FACTURA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\doc_masiva\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E423C32-9482-4B18-B5C1-EA6F2D05FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210F882F-1457-40D2-A8EB-94F5F0AFEFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-1425" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{3CEB5654-8E3F-48D9-A6B5-228D6F666F27}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="123">
   <si>
     <t xml:space="preserve">Inicializar variables </t>
   </si>
@@ -638,6 +638,18 @@
   </si>
   <si>
     <t>obtener_nuis_disponibles()</t>
+  </si>
+  <si>
+    <t>obtener_nombre_usuario()</t>
+  </si>
+  <si>
+    <t>genera el nombre de usuario que se va a registrar en los campos CREATED_BY de cada tabla afectada</t>
+  </si>
+  <si>
+    <t>obtener_cedis_x_remitente()</t>
+  </si>
+  <si>
+    <t>obtiene el CEDIS que corresponda al remitente</t>
   </si>
 </sst>
 </file>
@@ -1054,6 +1066,21 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1065,21 +1092,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1495,7 +1507,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1506,7 +1518,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
@@ -1520,7 +1532,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="40" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1531,7 +1543,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1548,7 +1560,7 @@
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="39" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1559,7 +1571,7 @@
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1589,11 +1601,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1674,7 +1686,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="39" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -1685,7 +1697,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="7" t="s">
         <v>52</v>
       </c>
@@ -1751,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267302D1-1807-4EAE-9A86-AD84416E3204}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1767,10 +1779,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="42"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -2040,16 +2052,16 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="39">
+      <c r="A23" s="35">
         <v>19</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="37"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
@@ -2147,7 +2159,35 @@
       <c r="C31" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="42" t="s">
+      <c r="D31" s="38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="23">
+        <v>28</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="23">
+        <v>29</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="38" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>